<commit_message>
MaxPowerLevel, MaxStageLevel 인트키 추가
각 샷의 대미지 보정인 DamageRateTable 추가
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7C6C35-36F7-4DA7-BA84-D74D7596FB7A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2688ACD7-6B4A-4360-B0A4-A41B634C71CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
     <sheet name="GlobalConstantFloatTable" sheetId="2" r:id="rId2"/>
+    <sheet name="DamageRateTable" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,16 +32,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>id|String</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GlobalConstant_MaxRank</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>value|Float</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -50,6 +47,73 @@
   </si>
   <si>
     <t>SpDecreaseRate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxStageLevel</t>
+  </si>
+  <si>
+    <t>MaxPowerLevel</t>
+  </si>
+  <si>
+    <t>id|String</t>
+  </si>
+  <si>
+    <t>number|Int</t>
+  </si>
+  <si>
+    <t>Ricochet</t>
+  </si>
+  <si>
+    <t>1,0.7</t>
+  </si>
+  <si>
+    <t>1,0.7,0.49</t>
+  </si>
+  <si>
+    <t>1,0.7,0.2</t>
+  </si>
+  <si>
+    <t>BounceWallQuad</t>
+  </si>
+  <si>
+    <t>1,0.5</t>
+  </si>
+  <si>
+    <t>1,0.5,0.25</t>
+  </si>
+  <si>
+    <t>MonsterThrough</t>
+  </si>
+  <si>
+    <t>1,0.66</t>
+  </si>
+  <si>
+    <t>1,0.66,0.3</t>
+  </si>
+  <si>
+    <t>Repeat</t>
+  </si>
+  <si>
+    <t>1,0.9</t>
+  </si>
+  <si>
+    <t>1,0.9,0.81</t>
+  </si>
+  <si>
+    <t>1.0.9,0.72</t>
+  </si>
+  <si>
+    <t>Parallel</t>
+  </si>
+  <si>
+    <t>CircularSector</t>
+  </si>
+  <si>
+    <t>WallThrough</t>
+  </si>
+  <si>
+    <t>rate|Float!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -414,6 +478,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BB9F1B-6CB9-4C59-8005-03A25A60D336}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34769A5-C368-4A5A-B8DE-2FA85EFEC3A4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -428,15 +533,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -445,31 +550,177 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34769A5-C368-4A5A-B8DE-2FA85EFEC3A4}">
-  <dimension ref="A1:B2"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C64605-056A-4FEA-8334-385AFFA75F0F}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.75" customWidth="1"/>
+    <col min="1" max="1" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
         <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GlobalConstant 엑셀의 GlobalConstantStringTable 테이블 추가
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A51DB8-33C0-4230-AB3D-E68573AA161C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD422BAB-0276-47FA-A984-7E8564A56FAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
+    <workbookView xWindow="-16050" yWindow="3825" windowWidth="14025" windowHeight="10680" firstSheet="1" activeTab="2" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>id|String</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,30 +85,6 @@
     <t>value|String</t>
   </si>
   <si>
-    <t>DropHealAffectorValueId</t>
-  </si>
-  <si>
-    <t>LevelUpHealAffectorValueId</t>
-  </si>
-  <si>
-    <t>SwapHealAffectorValueId</t>
-  </si>
-  <si>
-    <t>PowerSourceHealAffectorValueId</t>
-  </si>
-  <si>
-    <t>PowerSourceMagicBuffAffectorValueId</t>
-  </si>
-  <si>
-    <t>PowerSourceMachineBuffAffectorValueId</t>
-  </si>
-  <si>
-    <t>PowerSourceNatureBuffAffectorValueId</t>
-  </si>
-  <si>
-    <t>PowerSourceQigongBuffAffectorValueId</t>
-  </si>
-  <si>
     <t>rate|Float!</t>
   </si>
   <si>
@@ -143,6 +119,13 @@
   </si>
   <si>
     <t>CollisionDamageInterval</t>
+  </si>
+  <si>
+    <t>MaxHpBetter</t>
+  </si>
+  <si>
+    <t>ExclusiveLevelPackIdAfterMax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -549,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34769A5-C368-4A5A-B8DE-2FA85EFEC3A4}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -584,7 +567,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>0.9</v>
@@ -598,13 +581,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377D5FC1-6BFD-4414-8A0B-4D8B6A8A7BBB}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -617,42 +601,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>22</v>
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -683,7 +635,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -694,7 +646,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -705,7 +657,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -716,7 +668,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -727,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -738,7 +690,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -749,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -760,7 +712,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -771,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -782,7 +734,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -793,7 +745,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
TutorialStartX, TutorialStartZ 글로벌컨트턴트플롯테이블에 추가 임시값 -1.5, -3
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA452590-FBEC-4BB3-8FFF-13C504A3D46C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDA6FBA-1409-4218-AE06-4EE43960DF37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>MaxStageLevel</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>MaxTutorialStage</t>
+  </si>
+  <si>
+    <t>TutorialStartX</t>
+  </si>
+  <si>
+    <t>TutorialStartZ</t>
   </si>
 </sst>
 </file>
@@ -540,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BB9F1B-6CB9-4C59-8005-03A25A60D336}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -605,9 +611,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34769A5-C368-4A5A-B8DE-2FA85EFEC3A4}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -724,6 +732,22 @@
       </c>
       <c r="B14">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16">
+        <v>-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TimeSecToGetOneEnergy RequiredEnergyToPlay RefillEnergyDiamond 상수 3개 추가
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890292A7-0425-4647-AC35-FE8EE5ADD0FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ED6424-E8E7-40CF-BBEC-5CE0A1808B4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>MaxStageLevel</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>MaxTutorialStage</t>
+  </si>
+  <si>
+    <t>TimeSecToGetOneEnergy</t>
+  </si>
+  <si>
+    <t>RequiredEnergyToPlay</t>
+  </si>
+  <si>
+    <t>RefillEnergyDiamond</t>
   </si>
 </sst>
 </file>
@@ -538,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BB9F1B-6CB9-4C59-8005-03A25A60D336}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -597,6 +606,30 @@
         <v>30</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -607,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34769A5-C368-4A5A-B8DE-2FA85EFEC3A4}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
초월 공드 비용 3단계 추가 TranscendGoldOne, Two, Three
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198C2F9A-1B9D-48EB-A426-B994A455E1EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349428C4-817C-48D8-AA41-FF448C10FC4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
   <si>
     <t>MaxStageLevel</t>
   </si>
@@ -247,6 +247,15 @@
   </si>
   <si>
     <t>1,0.4</t>
+  </si>
+  <si>
+    <t>TranscendGoldOne</t>
+  </si>
+  <si>
+    <t>TranscendGoldTwo</t>
+  </si>
+  <si>
+    <t>TranscendGoldThree</t>
   </si>
 </sst>
 </file>
@@ -610,9 +619,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BB9F1B-6CB9-4C59-8005-03A25A60D336}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -801,6 +812,30 @@
       </c>
       <c r="B23">
         <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26">
+        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MaxGuideQuestId 임시값 4 추가
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268A5AD8-D8FE-415E-A4BA-8985A56F44EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55488C1B-11E7-4D8F-98ED-14E5984E8950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
   <si>
     <t>MaxStageLevel</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>1,0.46,0.21,0.1</t>
+  </si>
+  <si>
+    <t>MaxGuideQuestId</t>
   </si>
 </sst>
 </file>
@@ -655,7 +658,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BB9F1B-6CB9-4C59-8005-03A25A60D336}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -944,6 +947,14 @@
       </c>
       <c r="B35">
         <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
노드워 50 => 100 클라 상수 조정 드랍 힐 0.17 => 0.16
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7361E85-ECBB-4E42-BEAA-23BD4C9F7C28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9833730-8AEE-476D-97AD-778256A84BB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -738,7 +738,7 @@
         <v>48</v>
       </c>
       <c r="B6">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1055,7 +1055,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34769A5-C368-4A5A-B8DE-2FA85EFEC3A4}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1107,7 +1109,7 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
드랍 힐 0.16 => 0.15 조정
</commit_message>
<xml_diff>
--- a/Excel/GlobalConstant.xlsx
+++ b/Excel/GlobalConstant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350D355B-72C8-416D-A58D-0BE487DFF66D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D666E394-0133-4EA9-8356-45BA13D8AF6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4D719337-7574-466E-8B01-73E036BA373F}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalConstantIntTable" sheetId="1" r:id="rId1"/>
@@ -687,385 +687,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BB9F1B-6CB9-4C59-8005-03A25A60D336}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="24.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>86</v>
-      </c>
-      <c r="B39">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>92</v>
-      </c>
-      <c r="B42">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>93</v>
-      </c>
-      <c r="B43">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>94</v>
-      </c>
-      <c r="B44">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>95</v>
-      </c>
-      <c r="B45">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34769A5-C368-4A5A-B8DE-2FA85EFEC3A4}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -1080,6 +701,383 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34769A5-C368-4A5A-B8DE-2FA85EFEC3A4}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1120,7 +1118,7 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>